<commit_message>
preparazione calcolo variabili tempo-dipendenti
</commit_message>
<xml_diff>
--- a/i_codebooks/D3_TD_condition.xlsx
+++ b/i_codebooks/D3_TD_condition.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20408"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Davide\Documents\Git repositories\Work\ROC18\i_codebooks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rosgin2\Documents\emorragie_gravi\i_codebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79C8F1FD-E12A-4A57-A1BF-DDEEFA79403B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -18,12 +17,12 @@
     <sheet name="Parameters" sheetId="3" r:id="rId3"/>
     <sheet name="Examples" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="41">
   <si>
     <t>medatata_name</t>
   </si>
@@ -37,12 +36,110 @@
     <t>Content of the dataset</t>
   </si>
   <si>
+    <t>Unit of observation</t>
+  </si>
+  <si>
+    <t>Dataset where the list of UoOs is fully listed and with 1 record per UoO</t>
+  </si>
+  <si>
+    <t>How many observations per UoO</t>
+  </si>
+  <si>
+    <t>Variables capturing the UoO</t>
+  </si>
+  <si>
+    <t>person_id</t>
+  </si>
+  <si>
+    <t>Primary key</t>
+  </si>
+  <si>
+    <t>person_id date value_of_variable</t>
+  </si>
+  <si>
+    <t>Parameters</t>
+  </si>
+  <si>
+    <t>VarName</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Format</t>
+  </si>
+  <si>
+    <t>Vocabulary</t>
+  </si>
+  <si>
+    <t>Notes and examples</t>
+  </si>
+  <si>
+    <t>Source tables and variables</t>
+  </si>
+  <si>
+    <t>Retrieved</t>
+  </si>
+  <si>
+    <t>Calculated</t>
+  </si>
+  <si>
+    <t>Algorithm_id</t>
+  </si>
+  <si>
+    <t>Rule</t>
+  </si>
+  <si>
+    <t>unique person identifier</t>
+  </si>
+  <si>
+    <t>character</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>date when the condition changes; the components of the condition last 365 days if they are diagnosis, and 90 days if they are drug proxies; unique spells are created when the algorithm is 1 (if either a dianosis or a drug proxy is active), and the algorithm is reverted to values 0 whenever no component is active</t>
+  </si>
+  <si>
+    <t>value_of_variable</t>
+  </si>
+  <si>
+    <t>binary</t>
+  </si>
+  <si>
+    <t>1 = at least one of the components of the algorithm that define the condition is active
+0 = otherwise</t>
+  </si>
+  <si>
+    <t>parameter in the variable name</t>
+  </si>
+  <si>
+    <t>values</t>
+  </si>
+  <si>
+    <t>name of macro</t>
+  </si>
+  <si>
+    <t>condition</t>
+  </si>
+  <si>
+    <t>D3_TD_condition</t>
+  </si>
+  <si>
+    <t>D3_source_population</t>
+  </si>
+  <si>
+    <t>a person in the source population</t>
+  </si>
+  <si>
+    <t>As many as the variation of the values of the variable from the moment the person enters to the moment the person exits the source population. Since the variable is expected to be non missing at any moment, the baseline value is recorded for all the units of observation</t>
+  </si>
+  <si>
     <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF444444"/>
-        <rFont val="Calibri"/>
-      </rPr>
       <t xml:space="preserve">contains the time-dependent evolution of the binary variable </t>
     </r>
     <r>
@@ -51,6 +148,7 @@
         <sz val="14"/>
         <color rgb="FF444444"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">condition. </t>
     </r>
@@ -59,211 +157,22 @@
         <sz val="14"/>
         <color rgb="FF444444"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
-      <t>Only changes of status are recorded, with date when the condition changes; the components of the condition last 365 days if they are diagnosis, and 90 days if they are drug proxies; unique spells are created when the algorithm is 1 (if either a dianosis or a drug proxy is active), and the algorithm is reverted to values 0 whenever no component is active</t>
+      <t>Only changes of status are recorded</t>
     </r>
   </si>
   <si>
-    <t>Unit of observation</t>
-  </si>
-  <si>
-    <t>a person in the readiness study population</t>
-  </si>
-  <si>
-    <t>Dataset where the list of UoOs is fully listed and with 1 record per UoO</t>
-  </si>
-  <si>
-    <t>D4_study_population</t>
-  </si>
-  <si>
-    <t>How many observations per UoO</t>
-  </si>
-  <si>
-    <t>As many as the variation of the values of the variable from the moment the person enters to the moment the person exits the data source. Since the variable is expected to be non missing at any moment, the baseline value is recorded for all the units of observation</t>
-  </si>
-  <si>
-    <t>Variables capturing the UoO</t>
-  </si>
-  <si>
-    <t>person_id</t>
-  </si>
-  <si>
-    <t>Primary key</t>
-  </si>
-  <si>
-    <t>person_id date value_of_variable</t>
-  </si>
-  <si>
-    <t>Parameters</t>
-  </si>
-  <si>
-    <t>VarName</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Format</t>
-  </si>
-  <si>
-    <t>Vocabulary</t>
-  </si>
-  <si>
-    <t>Notes and examples</t>
-  </si>
-  <si>
-    <t>Source tables and variables</t>
-  </si>
-  <si>
-    <t>Retrieved</t>
-  </si>
-  <si>
-    <t>Calculated</t>
-  </si>
-  <si>
-    <t>Algorithm_id</t>
-  </si>
-  <si>
-    <t>Rule</t>
-  </si>
-  <si>
-    <t>unique person identifier</t>
-  </si>
-  <si>
-    <t>character</t>
-  </si>
-  <si>
-    <t>from D4_study_population</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>date</t>
-  </si>
-  <si>
-    <t>date when the condition changes; the components of the condition last 365 days if they are diagnosis, and 90 days if they are drug proxies; unique spells are created when the algorithm is 1 (if either a dianosis or a drug proxy is active), and the algorithm is reverted to values 0 whenever no component is active</t>
-  </si>
-  <si>
-    <t>value_of_variable</t>
-  </si>
-  <si>
-    <t>binary</t>
-  </si>
-  <si>
-    <t>1 = at least one of the components of the algorithm that define the condition is active
-0 = otherwise</t>
-  </si>
-  <si>
-    <t>parameter in the variable name</t>
-  </si>
-  <si>
-    <t>values</t>
-  </si>
-  <si>
-    <t>name of macro</t>
-  </si>
-  <si>
-    <t>condition</t>
-  </si>
-  <si>
-    <t>DIAB</t>
-  </si>
-  <si>
-    <t>list_of_covariates_for_cohort</t>
-  </si>
-  <si>
-    <t>CANCER</t>
-  </si>
-  <si>
-    <t>PULMON</t>
-  </si>
-  <si>
-    <t>OBES</t>
-  </si>
-  <si>
-    <t>CKD</t>
-  </si>
-  <si>
-    <t>HIV</t>
-  </si>
-  <si>
-    <t>IMMUNOSUP</t>
-  </si>
-  <si>
-    <t>SICKLE</t>
-  </si>
-  <si>
-    <t>CVD</t>
-  </si>
-  <si>
-    <t>P0001</t>
-  </si>
-  <si>
-    <t>P0011</t>
-  </si>
-  <si>
-    <t>P0013</t>
-  </si>
-  <si>
-    <t>P0014</t>
-  </si>
-  <si>
-    <t>P0015</t>
-  </si>
-  <si>
-    <t>P0016</t>
-  </si>
-  <si>
-    <t>P0017</t>
-  </si>
-  <si>
-    <t>P0018</t>
-  </si>
-  <si>
-    <t>P0019</t>
-  </si>
-  <si>
-    <t>P0020</t>
-  </si>
-  <si>
-    <t>P0021</t>
-  </si>
-  <si>
-    <t>P0022</t>
-  </si>
-  <si>
-    <t>P0023</t>
-  </si>
-  <si>
-    <t>P0024</t>
-  </si>
-  <si>
-    <t>P0025</t>
-  </si>
-  <si>
-    <t>P0026</t>
-  </si>
-  <si>
-    <t>P0027</t>
-  </si>
-  <si>
-    <t>P0073</t>
-  </si>
-  <si>
-    <t>P0074</t>
-  </si>
-  <si>
-    <t>remark that P00074 gets back to 0 90 days after becoming 1</t>
-  </si>
-  <si>
-    <t>D3_TD_condition</t>
+    <t>from D3_source_population</t>
+  </si>
+  <si>
+    <t>TD_variables_condition</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
@@ -279,6 +188,7 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -298,12 +208,14 @@
       <sz val="14"/>
       <color rgb="FF444444"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
       <sz val="14"/>
       <color rgb="FF444444"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -333,33 +245,28 @@
       <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFCE4D6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -485,7 +392,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -511,15 +418,13 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -549,7 +454,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -860,20 +765,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="38.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="144.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="144.7265625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -881,68 +786,68 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="24" t="s">
+    <row r="2" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A2" s="22" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="75" x14ac:dyDescent="0.3">
-      <c r="A3" s="25" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A3" s="23" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A4" s="23" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="25" t="s">
+      <c r="B4" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="32" x14ac:dyDescent="0.45">
+      <c r="A5" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B5" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="55.5" x14ac:dyDescent="0.45">
+      <c r="A6" s="23" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" ht="32.25" x14ac:dyDescent="0.3">
-      <c r="A5" s="25" t="s">
+      <c r="B6" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A7" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B7" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="56.25" x14ac:dyDescent="0.3">
-      <c r="A6" s="25" t="s">
+    <row r="8" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A8" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B8" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="25" t="s">
+    <row r="9" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="26" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A10" s="9"/>
       <c r="B10" s="6"/>
     </row>
@@ -952,118 +857,118 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F3" sqref="F3"/>
+      <selection pane="bottomRight" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="21.7265625" style="2" customWidth="1"/>
     <col min="2" max="2" width="31" style="2" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7265625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="39" style="2" customWidth="1"/>
-    <col min="5" max="5" width="72.28515625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="29.85546875" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="2"/>
+    <col min="5" max="5" width="72.26953125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="29.81640625" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="9.1796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="G1" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="H1" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="I1" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" s="19" t="s">
+      <c r="J1" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="K1" s="20" t="s">
         <v>21</v>
-      </c>
-      <c r="H1" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="I1" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="J1" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="K1" s="22" t="s">
-        <v>25</v>
       </c>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
-      <c r="O1" s="23"/>
-      <c r="P1" s="23"/>
-      <c r="Q1" s="23"/>
-      <c r="R1" s="23"/>
-      <c r="S1" s="23"/>
-      <c r="T1" s="23"/>
-      <c r="U1" s="23"/>
-      <c r="V1" s="23"/>
-      <c r="W1" s="23"/>
-      <c r="X1" s="23"/>
-      <c r="Y1" s="23"/>
-      <c r="Z1" s="23"/>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="O1" s="21"/>
+      <c r="P1" s="21"/>
+      <c r="Q1" s="21"/>
+      <c r="R1" s="21"/>
+      <c r="S1" s="21"/>
+      <c r="T1" s="21"/>
+      <c r="U1" s="21"/>
+      <c r="V1" s="21"/>
+      <c r="W1" s="21"/>
+      <c r="X1" s="21"/>
+      <c r="Y1" s="21"/>
+      <c r="Z1" s="21"/>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="E2" s="3"/>
       <c r="H2" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="186" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="62" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="3" spans="1:26" ht="180" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" ht="60" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>34</v>
-      </c>
       <c r="I4" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1072,128 +977,68 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC9CBAAA-B217-47D4-A09E-8EEA9DD4FAA5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="A3" sqref="A3:D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="B1" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="C1" s="17" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="C3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="B4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="C5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="C6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="C7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="C8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="C9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="C10" t="s">
-        <v>40</v>
-      </c>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="10"/>
+      <c r="B3" s="11"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="10"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="10"/>
+      <c r="B5" s="11"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="10"/>
+      <c r="B6" s="11"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="10"/>
+      <c r="B7" s="11"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" s="10"/>
+      <c r="B8" s="11"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" s="10"/>
+      <c r="B9" s="11"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" s="10"/>
+      <c r="B10" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1201,293 +1046,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF08289F-052C-4A07-84C5-136721429E0A}">
-  <dimension ref="A1:C27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="A1:C27"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.140625" customWidth="1"/>
-    <col min="2" max="2" width="27.42578125" style="12" customWidth="1"/>
-    <col min="3" max="3" width="24.5703125" customWidth="1"/>
-    <col min="4" max="4" width="26.28515625" customWidth="1"/>
-    <col min="5" max="5" width="26.7109375" customWidth="1"/>
+    <col min="1" max="1" width="19.1796875" customWidth="1"/>
+    <col min="2" max="2" width="27.453125" style="12" customWidth="1"/>
+    <col min="3" max="3" width="24.54296875" customWidth="1"/>
+    <col min="4" max="4" width="26.26953125" customWidth="1"/>
+    <col min="5" max="5" width="26.7265625" customWidth="1"/>
     <col min="6" max="6" width="24" customWidth="1"/>
   </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="C1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B2" s="12">
-        <v>43466</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B3" s="12">
-        <v>43466</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B4" s="12">
-        <v>43466</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B5" s="12">
-        <v>43466</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>53</v>
-      </c>
-      <c r="B6" s="12">
-        <v>43466</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>54</v>
-      </c>
-      <c r="B7" s="12">
-        <v>43466</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>55</v>
-      </c>
-      <c r="B8" s="12">
-        <v>43466</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="B9" s="14">
-        <v>43466</v>
-      </c>
-      <c r="C9" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="B10" s="14">
-        <v>44212</v>
-      </c>
-      <c r="C10" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>57</v>
-      </c>
-      <c r="B11" s="12">
-        <v>43466</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>58</v>
-      </c>
-      <c r="B12" s="12">
-        <v>43466</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>59</v>
-      </c>
-      <c r="B13" s="12">
-        <v>43466</v>
-      </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>60</v>
-      </c>
-      <c r="B14" s="12">
-        <v>43466</v>
-      </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>61</v>
-      </c>
-      <c r="B15" s="12">
-        <v>43466</v>
-      </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="B16" s="14">
-        <v>43635</v>
-      </c>
-      <c r="C16" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="B17" s="14">
-        <v>44223</v>
-      </c>
-      <c r="C17" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>63</v>
-      </c>
-      <c r="B18" s="12">
-        <v>43466</v>
-      </c>
-      <c r="C18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>64</v>
-      </c>
-      <c r="B19" s="12">
-        <v>43466</v>
-      </c>
-      <c r="C19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>65</v>
-      </c>
-      <c r="B20" s="12">
-        <v>43466</v>
-      </c>
-      <c r="C20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>66</v>
-      </c>
-      <c r="B21" s="12">
-        <v>43466</v>
-      </c>
-      <c r="C21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="B22" s="14">
-        <v>43924</v>
-      </c>
-      <c r="C22" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="B23" s="14">
-        <v>44208</v>
-      </c>
-      <c r="C23" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="B24" s="14">
-        <v>44299</v>
-      </c>
-      <c r="C24" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C27" t="s">
-        <v>68</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <sortState ref="A2:C23">
     <sortCondition ref="A2:A23"/>
     <sortCondition ref="B2:B23"/>
@@ -1497,15 +1070,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Comments xmlns="8029070a-695f-410c-a424-24d0683063af" xsi:nil="true"/>
-    <TaxCatchAll xmlns="797b3a1e-a17b-4ca2-8e72-b47fcb862c81" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8029070a-695f-410c-a424-24d0683063af">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1760,21 +1330,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Comments xmlns="8029070a-695f-410c-a424-24d0683063af" xsi:nil="true"/>
+    <TaxCatchAll xmlns="797b3a1e-a17b-4ca2-8e72-b47fcb862c81" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8029070a-695f-410c-a424-24d0683063af">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE8A1FD8-B49B-4DD5-B035-18D91695717A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E3594D7-89C9-4FB7-87F1-388B97141296}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="8029070a-695f-410c-a424-24d0683063af"/>
-    <ds:schemaRef ds:uri="797b3a1e-a17b-4ca2-8e72-b47fcb862c81"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1799,9 +1369,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E3594D7-89C9-4FB7-87F1-388B97141296}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE8A1FD8-B49B-4DD5-B035-18D91695717A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="8029070a-695f-410c-a424-24d0683063af"/>
+    <ds:schemaRef ds:uri="797b3a1e-a17b-4ca2-8e72-b47fcb862c81"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>